<commit_message>
Adaugat CEC si Raiffaisen
</commit_message>
<xml_diff>
--- a/Lista_banci.xlsx
+++ b/Lista_banci.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>Nume</t>
   </si>
@@ -121,6 +121,26 @@
   </si>
   <si>
     <t>90 euro</t>
+  </si>
+  <si>
+    <t>2.75%+IRCC</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>CEC Bank
+Fara credit prin card</t>
+  </si>
+  <si>
+    <t>CEC Bank
+Cu credit prin card</t>
+  </si>
+  <si>
+    <t>2.15%+IRCC</t>
+  </si>
+  <si>
+    <t>1.90%+IRCC</t>
   </si>
 </sst>
 </file>
@@ -478,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q7"/>
+  <dimension ref="B2:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,6 +780,15 @@
       <c r="G7" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K7" s="5">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -774,6 +803,133 @@
       </c>
       <c r="O7" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="1">
+        <f>M7/L7*100</f>
+        <v>220.61755952380952</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1">
+        <v>900</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="5">
+        <v>5.9200000000000003E-2</v>
+      </c>
+      <c r="L8" s="1">
+        <v>336000</v>
+      </c>
+      <c r="M8" s="1">
+        <v>705782</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1900</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>M8/L8*100</f>
+        <v>210.05416666666665</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1">
+        <v>500</v>
+      </c>
+      <c r="E9" s="1">
+        <v>134</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="1">
+        <v>336000</v>
+      </c>
+      <c r="M9" s="1">
+        <v>682193</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1900</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="1">
+        <f>M9/L9*100</f>
+        <v>203.03363095238095</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1">
+        <v>500</v>
+      </c>
+      <c r="E10" s="1">
+        <v>134</v>
+      </c>
+      <c r="L10" s="1">
+        <v>336000</v>
+      </c>
+      <c r="M10" s="1">
+        <v>663884</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1848</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="1">
+        <f>M10/L10*100</f>
+        <v>197.5845238095238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>